<commit_message>
Add support for creating substrings in TextRange. Update task list.
</commit_message>
<xml_diff>
--- a/docs/task-list.xlsx
+++ b/docs/task-list.xlsx
@@ -539,7 +539,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -550,7 +550,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -625,7 +625,10 @@
         <v>7</v>
       </c>
       <c r="F3" s="3">
-        <v>42037</v>
+        <v>42036</v>
+      </c>
+      <c r="G3" s="3">
+        <v>37302</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update task list in project
</commit_message>
<xml_diff>
--- a/docs/task-list.xlsx
+++ b/docs/task-list.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="8130"/>
   </bookViews>
   <sheets>
-    <sheet name="Task list" sheetId="1" r:id="rId1"/>
+    <sheet name="Task list - Core library" sheetId="1" r:id="rId1"/>
     <sheet name="Project Summary" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
   <si>
     <t>Description</t>
   </si>
@@ -49,9 +49,6 @@
     <t>high</t>
   </si>
   <si>
-    <t>Tasks</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Add support for editing existing text in </t>
     </r>
@@ -112,6 +109,100 @@
   </si>
   <si>
     <t>TextRange should support to create substring feature in text documents.</t>
+  </si>
+  <si>
+    <t>normal</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>TextDocument</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> should handle duplicated </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>TextRanges</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">When we register or create a new </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>TextRange</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> then </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>TextDocument</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> should check its existence to avoid duplications</t>
+    </r>
+  </si>
+  <si>
+    <t>done</t>
   </si>
 </sst>
 </file>
@@ -539,7 +630,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -547,10 +638,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="A3" sqref="A3:G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -596,10 +687,10 @@
         <v>8</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>10</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>11</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>7</v>
@@ -616,19 +707,42 @@
         <v>8</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>13</v>
-      </c>
       <c r="E3" s="2" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="F3" s="3">
         <v>42036</v>
       </c>
       <c r="G3" s="3">
         <v>37302</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="3">
+        <v>42041</v>
+      </c>
+      <c r="G4" s="3">
+        <v>42041</v>
       </c>
     </row>
   </sheetData>
@@ -664,18 +778,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update task list of project
</commit_message>
<xml_diff>
--- a/docs/task-list.xlsx
+++ b/docs/task-list.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="28">
   <si>
     <t>Description</t>
   </si>
@@ -43,9 +43,6 @@
     <t>Progress</t>
   </si>
   <si>
-    <t>in-progress</t>
-  </si>
-  <si>
     <t>high</t>
   </si>
   <si>
@@ -151,6 +148,80 @@
     </r>
   </si>
   <si>
+    <t>done</t>
+  </si>
+  <si>
+    <t>low</t>
+  </si>
+  <si>
+    <t>to-do</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Remove </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>TextRange</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>TextDocument</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> should support removing text ranges from list. TextDocument should have a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>TextDocument.RemoveTextRange</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> method for this feature.</t>
+    </r>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">When we register or create a new </t>
     </r>
@@ -198,11 +269,107 @@
         <charset val="238"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> should check its existence to avoid duplications</t>
-    </r>
-  </si>
-  <si>
-    <t>done</t>
+      <t xml:space="preserve"> should check its existence to avoid duplications.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Create a stub visitor for </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CSV</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> language</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">There should be a stub visitor for testing </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CSV</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> grammar.</t>
+    </r>
+  </si>
+  <si>
+    <t>There should be a factory for creating CSV node and it should build syntax and semantic tree as well</t>
+  </si>
+  <si>
+    <t>Implement semantic trees and nodes</t>
+  </si>
+  <si>
+    <t>There should be implemented semantic nodes and trees data structure beside nodes</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Implement a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CSV tree factory</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> for reduce dependency</t>
+    </r>
+  </si>
+  <si>
+    <t>Reconsider SelectRelativeNodesOperand implementation</t>
+  </si>
+  <si>
+    <t>When algorithm finds a proper valid node it should not continue search in its children</t>
   </si>
 </sst>
 </file>
@@ -232,12 +399,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -252,7 +431,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -270,6 +449,24 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -630,7 +827,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -638,10 +835,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:G4"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -680,69 +877,175 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+      <c r="A2" s="7">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="3">
+      <c r="E2" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="11">
         <v>42036</v>
+      </c>
+      <c r="G2" s="11">
+        <v>42044</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
+      <c r="A3" s="7">
         <v>2</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="4" t="s">
+      <c r="B3" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="3">
+      <c r="E3" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="11">
         <v>42036</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3" s="11">
         <v>37302</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
+      <c r="A4" s="7">
         <v>3</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="D4" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="F4" s="11">
+        <v>42041</v>
+      </c>
+      <c r="G4" s="11">
+        <v>42041</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="C5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="3">
-        <v>42041</v>
-      </c>
-      <c r="G4" s="3">
-        <v>42041</v>
+      <c r="F5" s="3">
+        <v>42044</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="3">
+        <v>42044</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="11">
+        <v>42049</v>
+      </c>
+      <c r="G7" s="11">
+        <v>42049</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="3">
+        <v>42049</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="3">
+        <v>42050</v>
       </c>
     </row>
   </sheetData>
@@ -762,7 +1065,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576">
       <formula1>"normal,low,high"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E7">
       <formula1>"to-do,in-progress,done"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Make some refactoring in Nodes folder
</commit_message>
<xml_diff>
--- a/docs/task-list.xlsx
+++ b/docs/task-list.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="30">
   <si>
     <t>Description</t>
   </si>
@@ -370,6 +370,37 @@
   </si>
   <si>
     <t>When algorithm finds a proper valid node it should not continue search in its children</t>
+  </si>
+  <si>
+    <t>Implement an error handling logic to the whole application</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">There should be a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Protect</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">-like method for handling errors and every exception should be caught. </t>
+    </r>
   </si>
 </sst>
 </file>
@@ -827,7 +858,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -835,10 +866,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1046,6 +1077,26 @@
       </c>
       <c r="F9" s="3">
         <v>42050</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="3">
+        <v>42059</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Make some refactoring and renaming of classes
</commit_message>
<xml_diff>
--- a/docs/task-list.xlsx
+++ b/docs/task-list.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="35">
   <si>
     <t>Description</t>
   </si>
@@ -400,6 +400,114 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">-like method for handling errors and every exception should be caught. </t>
+    </r>
+  </si>
+  <si>
+    <t>Support 2D text ranges</t>
+  </si>
+  <si>
+    <t>It should support 2D text ranges for rectangular selection of texts</t>
+  </si>
+  <si>
+    <t>in-progress</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CsvCompiler</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> class doesn't support </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dependency injection</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. Its Parse method or constructor should be extended. Dependencies should be tree visitors</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Add </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DI support</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CsvCompiler</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> class</t>
     </r>
   </si>
 </sst>
@@ -858,7 +966,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -866,10 +974,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G515"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -997,23 +1105,26 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
+      <c r="A6" s="7">
         <v>5</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" s="3">
+      <c r="E6" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="11">
         <v>42044</v>
+      </c>
+      <c r="G6" s="11">
+        <v>42066</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1052,7 +1163,7 @@
       <c r="D8" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="12" t="s">
         <v>16</v>
       </c>
       <c r="F8" s="3">
@@ -1072,7 +1183,7 @@
       <c r="D9" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="12" t="s">
         <v>16</v>
       </c>
       <c r="F9" s="3">
@@ -1092,12 +1203,1558 @@
       <c r="D10" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="12" t="s">
         <v>16</v>
       </c>
       <c r="F10" s="3">
         <v>42059</v>
       </c>
+    </row>
+    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="3">
+        <v>42066</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E13" s="12"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E14" s="12"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E15" s="12"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E16" s="12"/>
+    </row>
+    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E17" s="12"/>
+    </row>
+    <row r="18" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E18" s="12"/>
+    </row>
+    <row r="19" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E19" s="12"/>
+    </row>
+    <row r="20" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E20" s="12"/>
+    </row>
+    <row r="21" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E21" s="12"/>
+    </row>
+    <row r="22" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E22" s="12"/>
+    </row>
+    <row r="23" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E23" s="12"/>
+    </row>
+    <row r="24" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E24" s="12"/>
+    </row>
+    <row r="25" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E25" s="12"/>
+    </row>
+    <row r="26" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E26" s="12"/>
+    </row>
+    <row r="27" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E27" s="12"/>
+    </row>
+    <row r="28" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E28" s="12"/>
+    </row>
+    <row r="29" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E29" s="12"/>
+    </row>
+    <row r="30" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E30" s="12"/>
+    </row>
+    <row r="31" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E31" s="12"/>
+    </row>
+    <row r="32" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E32" s="12"/>
+    </row>
+    <row r="33" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E33" s="12"/>
+    </row>
+    <row r="34" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E34" s="12"/>
+    </row>
+    <row r="35" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E35" s="12"/>
+    </row>
+    <row r="36" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E36" s="12"/>
+    </row>
+    <row r="37" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E37" s="12"/>
+    </row>
+    <row r="38" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E38" s="12"/>
+    </row>
+    <row r="39" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E39" s="12"/>
+    </row>
+    <row r="40" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E40" s="12"/>
+    </row>
+    <row r="41" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E41" s="12"/>
+    </row>
+    <row r="42" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E42" s="12"/>
+    </row>
+    <row r="43" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E43" s="12"/>
+    </row>
+    <row r="44" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E44" s="12"/>
+    </row>
+    <row r="45" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E45" s="12"/>
+    </row>
+    <row r="46" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E46" s="12"/>
+    </row>
+    <row r="47" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E47" s="12"/>
+    </row>
+    <row r="48" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E48" s="12"/>
+    </row>
+    <row r="49" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E49" s="12"/>
+    </row>
+    <row r="50" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E50" s="12"/>
+    </row>
+    <row r="51" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E51" s="12"/>
+    </row>
+    <row r="52" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E52" s="12"/>
+    </row>
+    <row r="53" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E53" s="12"/>
+    </row>
+    <row r="54" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E54" s="12"/>
+    </row>
+    <row r="55" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E55" s="12"/>
+    </row>
+    <row r="56" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E56" s="12"/>
+    </row>
+    <row r="57" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E57" s="12"/>
+    </row>
+    <row r="58" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E58" s="12"/>
+    </row>
+    <row r="59" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E59" s="12"/>
+    </row>
+    <row r="60" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E60" s="12"/>
+    </row>
+    <row r="61" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E61" s="12"/>
+    </row>
+    <row r="62" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E62" s="12"/>
+    </row>
+    <row r="63" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E63" s="12"/>
+    </row>
+    <row r="64" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E64" s="12"/>
+    </row>
+    <row r="65" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E65" s="12"/>
+    </row>
+    <row r="66" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E66" s="12"/>
+    </row>
+    <row r="67" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E67" s="12"/>
+    </row>
+    <row r="68" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E68" s="12"/>
+    </row>
+    <row r="69" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E69" s="12"/>
+    </row>
+    <row r="70" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E70" s="12"/>
+    </row>
+    <row r="71" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E71" s="12"/>
+    </row>
+    <row r="72" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E72" s="12"/>
+    </row>
+    <row r="73" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E73" s="12"/>
+    </row>
+    <row r="74" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E74" s="12"/>
+    </row>
+    <row r="75" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E75" s="12"/>
+    </row>
+    <row r="76" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E76" s="12"/>
+    </row>
+    <row r="77" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E77" s="12"/>
+    </row>
+    <row r="78" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E78" s="12"/>
+    </row>
+    <row r="79" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E79" s="12"/>
+    </row>
+    <row r="80" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E80" s="12"/>
+    </row>
+    <row r="81" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E81" s="12"/>
+    </row>
+    <row r="82" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E82" s="12"/>
+    </row>
+    <row r="83" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E83" s="12"/>
+    </row>
+    <row r="84" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E84" s="12"/>
+    </row>
+    <row r="85" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E85" s="12"/>
+    </row>
+    <row r="86" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E86" s="12"/>
+    </row>
+    <row r="87" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E87" s="12"/>
+    </row>
+    <row r="88" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E88" s="12"/>
+    </row>
+    <row r="89" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E89" s="12"/>
+    </row>
+    <row r="90" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E90" s="12"/>
+    </row>
+    <row r="91" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E91" s="12"/>
+    </row>
+    <row r="92" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E92" s="12"/>
+    </row>
+    <row r="93" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E93" s="12"/>
+    </row>
+    <row r="94" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E94" s="12"/>
+    </row>
+    <row r="95" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E95" s="12"/>
+    </row>
+    <row r="96" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E96" s="12"/>
+    </row>
+    <row r="97" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E97" s="12"/>
+    </row>
+    <row r="98" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E98" s="12"/>
+    </row>
+    <row r="99" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E99" s="12"/>
+    </row>
+    <row r="100" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E100" s="12"/>
+    </row>
+    <row r="101" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E101" s="12"/>
+    </row>
+    <row r="102" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E102" s="12"/>
+    </row>
+    <row r="103" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E103" s="12"/>
+    </row>
+    <row r="104" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E104" s="12"/>
+    </row>
+    <row r="105" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E105" s="12"/>
+    </row>
+    <row r="106" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E106" s="12"/>
+    </row>
+    <row r="107" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E107" s="12"/>
+    </row>
+    <row r="108" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E108" s="12"/>
+    </row>
+    <row r="109" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E109" s="12"/>
+    </row>
+    <row r="110" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E110" s="12"/>
+    </row>
+    <row r="111" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E111" s="12"/>
+    </row>
+    <row r="112" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E112" s="12"/>
+    </row>
+    <row r="113" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E113" s="12"/>
+    </row>
+    <row r="114" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E114" s="12"/>
+    </row>
+    <row r="115" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E115" s="12"/>
+    </row>
+    <row r="116" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E116" s="12"/>
+    </row>
+    <row r="117" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E117" s="12"/>
+    </row>
+    <row r="118" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E118" s="12"/>
+    </row>
+    <row r="119" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E119" s="12"/>
+    </row>
+    <row r="120" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E120" s="12"/>
+    </row>
+    <row r="121" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E121" s="12"/>
+    </row>
+    <row r="122" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E122" s="12"/>
+    </row>
+    <row r="123" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E123" s="12"/>
+    </row>
+    <row r="124" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E124" s="12"/>
+    </row>
+    <row r="125" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E125" s="12"/>
+    </row>
+    <row r="126" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E126" s="12"/>
+    </row>
+    <row r="127" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E127" s="12"/>
+    </row>
+    <row r="128" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E128" s="12"/>
+    </row>
+    <row r="129" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E129" s="12"/>
+    </row>
+    <row r="130" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E130" s="12"/>
+    </row>
+    <row r="131" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E131" s="12"/>
+    </row>
+    <row r="132" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E132" s="12"/>
+    </row>
+    <row r="133" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E133" s="12"/>
+    </row>
+    <row r="134" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E134" s="12"/>
+    </row>
+    <row r="135" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E135" s="12"/>
+    </row>
+    <row r="136" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E136" s="12"/>
+    </row>
+    <row r="137" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E137" s="12"/>
+    </row>
+    <row r="138" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E138" s="12"/>
+    </row>
+    <row r="139" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E139" s="12"/>
+    </row>
+    <row r="140" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E140" s="12"/>
+    </row>
+    <row r="141" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E141" s="12"/>
+    </row>
+    <row r="142" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E142" s="12"/>
+    </row>
+    <row r="143" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E143" s="12"/>
+    </row>
+    <row r="144" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E144" s="12"/>
+    </row>
+    <row r="145" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E145" s="12"/>
+    </row>
+    <row r="146" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E146" s="12"/>
+    </row>
+    <row r="147" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E147" s="12"/>
+    </row>
+    <row r="148" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E148" s="12"/>
+    </row>
+    <row r="149" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E149" s="12"/>
+    </row>
+    <row r="150" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E150" s="12"/>
+    </row>
+    <row r="151" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E151" s="12"/>
+    </row>
+    <row r="152" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E152" s="12"/>
+    </row>
+    <row r="153" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E153" s="12"/>
+    </row>
+    <row r="154" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E154" s="12"/>
+    </row>
+    <row r="155" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E155" s="12"/>
+    </row>
+    <row r="156" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E156" s="12"/>
+    </row>
+    <row r="157" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E157" s="12"/>
+    </row>
+    <row r="158" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E158" s="12"/>
+    </row>
+    <row r="159" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E159" s="12"/>
+    </row>
+    <row r="160" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E160" s="12"/>
+    </row>
+    <row r="161" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E161" s="12"/>
+    </row>
+    <row r="162" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E162" s="12"/>
+    </row>
+    <row r="163" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E163" s="12"/>
+    </row>
+    <row r="164" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E164" s="12"/>
+    </row>
+    <row r="165" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E165" s="12"/>
+    </row>
+    <row r="166" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E166" s="12"/>
+    </row>
+    <row r="167" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E167" s="12"/>
+    </row>
+    <row r="168" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E168" s="12"/>
+    </row>
+    <row r="169" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E169" s="12"/>
+    </row>
+    <row r="170" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E170" s="12"/>
+    </row>
+    <row r="171" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E171" s="12"/>
+    </row>
+    <row r="172" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E172" s="12"/>
+    </row>
+    <row r="173" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E173" s="12"/>
+    </row>
+    <row r="174" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E174" s="12"/>
+    </row>
+    <row r="175" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E175" s="12"/>
+    </row>
+    <row r="176" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E176" s="12"/>
+    </row>
+    <row r="177" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E177" s="12"/>
+    </row>
+    <row r="178" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E178" s="12"/>
+    </row>
+    <row r="179" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E179" s="12"/>
+    </row>
+    <row r="180" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E180" s="12"/>
+    </row>
+    <row r="181" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E181" s="12"/>
+    </row>
+    <row r="182" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E182" s="12"/>
+    </row>
+    <row r="183" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E183" s="12"/>
+    </row>
+    <row r="184" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E184" s="12"/>
+    </row>
+    <row r="185" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E185" s="12"/>
+    </row>
+    <row r="186" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E186" s="12"/>
+    </row>
+    <row r="187" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E187" s="12"/>
+    </row>
+    <row r="188" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E188" s="12"/>
+    </row>
+    <row r="189" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E189" s="12"/>
+    </row>
+    <row r="190" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E190" s="12"/>
+    </row>
+    <row r="191" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E191" s="12"/>
+    </row>
+    <row r="192" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E192" s="12"/>
+    </row>
+    <row r="193" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E193" s="12"/>
+    </row>
+    <row r="194" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E194" s="12"/>
+    </row>
+    <row r="195" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E195" s="12"/>
+    </row>
+    <row r="196" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E196" s="12"/>
+    </row>
+    <row r="197" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E197" s="12"/>
+    </row>
+    <row r="198" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E198" s="12"/>
+    </row>
+    <row r="199" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E199" s="12"/>
+    </row>
+    <row r="200" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E200" s="12"/>
+    </row>
+    <row r="201" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E201" s="12"/>
+    </row>
+    <row r="202" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E202" s="12"/>
+    </row>
+    <row r="203" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E203" s="12"/>
+    </row>
+    <row r="204" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E204" s="12"/>
+    </row>
+    <row r="205" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E205" s="12"/>
+    </row>
+    <row r="206" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E206" s="12"/>
+    </row>
+    <row r="207" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E207" s="12"/>
+    </row>
+    <row r="208" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E208" s="12"/>
+    </row>
+    <row r="209" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E209" s="12"/>
+    </row>
+    <row r="210" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E210" s="12"/>
+    </row>
+    <row r="211" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E211" s="12"/>
+    </row>
+    <row r="212" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E212" s="12"/>
+    </row>
+    <row r="213" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E213" s="12"/>
+    </row>
+    <row r="214" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E214" s="12"/>
+    </row>
+    <row r="215" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E215" s="12"/>
+    </row>
+    <row r="216" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E216" s="12"/>
+    </row>
+    <row r="217" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E217" s="12"/>
+    </row>
+    <row r="218" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E218" s="12"/>
+    </row>
+    <row r="219" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E219" s="12"/>
+    </row>
+    <row r="220" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E220" s="12"/>
+    </row>
+    <row r="221" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E221" s="12"/>
+    </row>
+    <row r="222" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E222" s="12"/>
+    </row>
+    <row r="223" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E223" s="12"/>
+    </row>
+    <row r="224" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E224" s="12"/>
+    </row>
+    <row r="225" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E225" s="12"/>
+    </row>
+    <row r="226" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E226" s="12"/>
+    </row>
+    <row r="227" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E227" s="12"/>
+    </row>
+    <row r="228" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E228" s="12"/>
+    </row>
+    <row r="229" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E229" s="12"/>
+    </row>
+    <row r="230" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E230" s="12"/>
+    </row>
+    <row r="231" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E231" s="12"/>
+    </row>
+    <row r="232" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E232" s="12"/>
+    </row>
+    <row r="233" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E233" s="12"/>
+    </row>
+    <row r="234" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E234" s="12"/>
+    </row>
+    <row r="235" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E235" s="12"/>
+    </row>
+    <row r="236" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E236" s="12"/>
+    </row>
+    <row r="237" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E237" s="12"/>
+    </row>
+    <row r="238" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E238" s="12"/>
+    </row>
+    <row r="239" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E239" s="12"/>
+    </row>
+    <row r="240" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E240" s="12"/>
+    </row>
+    <row r="241" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E241" s="12"/>
+    </row>
+    <row r="242" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E242" s="12"/>
+    </row>
+    <row r="243" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E243" s="12"/>
+    </row>
+    <row r="244" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E244" s="12"/>
+    </row>
+    <row r="245" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E245" s="12"/>
+    </row>
+    <row r="246" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E246" s="12"/>
+    </row>
+    <row r="247" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E247" s="12"/>
+    </row>
+    <row r="248" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E248" s="12"/>
+    </row>
+    <row r="249" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E249" s="12"/>
+    </row>
+    <row r="250" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E250" s="12"/>
+    </row>
+    <row r="251" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E251" s="12"/>
+    </row>
+    <row r="252" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E252" s="12"/>
+    </row>
+    <row r="253" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E253" s="12"/>
+    </row>
+    <row r="254" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E254" s="12"/>
+    </row>
+    <row r="255" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E255" s="12"/>
+    </row>
+    <row r="256" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E256" s="12"/>
+    </row>
+    <row r="257" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E257" s="12"/>
+    </row>
+    <row r="258" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E258" s="12"/>
+    </row>
+    <row r="259" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E259" s="12"/>
+    </row>
+    <row r="260" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E260" s="12"/>
+    </row>
+    <row r="261" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E261" s="12"/>
+    </row>
+    <row r="262" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E262" s="12"/>
+    </row>
+    <row r="263" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E263" s="12"/>
+    </row>
+    <row r="264" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E264" s="12"/>
+    </row>
+    <row r="265" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E265" s="12"/>
+    </row>
+    <row r="266" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E266" s="12"/>
+    </row>
+    <row r="267" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E267" s="12"/>
+    </row>
+    <row r="268" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E268" s="12"/>
+    </row>
+    <row r="269" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E269" s="12"/>
+    </row>
+    <row r="270" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E270" s="12"/>
+    </row>
+    <row r="271" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E271" s="12"/>
+    </row>
+    <row r="272" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E272" s="12"/>
+    </row>
+    <row r="273" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E273" s="12"/>
+    </row>
+    <row r="274" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E274" s="12"/>
+    </row>
+    <row r="275" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E275" s="12"/>
+    </row>
+    <row r="276" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E276" s="12"/>
+    </row>
+    <row r="277" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E277" s="12"/>
+    </row>
+    <row r="278" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E278" s="12"/>
+    </row>
+    <row r="279" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E279" s="12"/>
+    </row>
+    <row r="280" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E280" s="12"/>
+    </row>
+    <row r="281" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E281" s="12"/>
+    </row>
+    <row r="282" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E282" s="12"/>
+    </row>
+    <row r="283" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E283" s="12"/>
+    </row>
+    <row r="284" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E284" s="12"/>
+    </row>
+    <row r="285" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E285" s="12"/>
+    </row>
+    <row r="286" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E286" s="12"/>
+    </row>
+    <row r="287" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E287" s="12"/>
+    </row>
+    <row r="288" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E288" s="12"/>
+    </row>
+    <row r="289" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E289" s="12"/>
+    </row>
+    <row r="290" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E290" s="12"/>
+    </row>
+    <row r="291" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E291" s="12"/>
+    </row>
+    <row r="292" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E292" s="12"/>
+    </row>
+    <row r="293" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E293" s="12"/>
+    </row>
+    <row r="294" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E294" s="12"/>
+    </row>
+    <row r="295" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E295" s="12"/>
+    </row>
+    <row r="296" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E296" s="12"/>
+    </row>
+    <row r="297" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E297" s="12"/>
+    </row>
+    <row r="298" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E298" s="12"/>
+    </row>
+    <row r="299" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E299" s="12"/>
+    </row>
+    <row r="300" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E300" s="12"/>
+    </row>
+    <row r="301" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E301" s="12"/>
+    </row>
+    <row r="302" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E302" s="12"/>
+    </row>
+    <row r="303" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E303" s="12"/>
+    </row>
+    <row r="304" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E304" s="12"/>
+    </row>
+    <row r="305" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E305" s="12"/>
+    </row>
+    <row r="306" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E306" s="12"/>
+    </row>
+    <row r="307" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E307" s="12"/>
+    </row>
+    <row r="308" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E308" s="12"/>
+    </row>
+    <row r="309" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E309" s="12"/>
+    </row>
+    <row r="310" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E310" s="12"/>
+    </row>
+    <row r="311" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E311" s="12"/>
+    </row>
+    <row r="312" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E312" s="12"/>
+    </row>
+    <row r="313" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E313" s="12"/>
+    </row>
+    <row r="314" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E314" s="12"/>
+    </row>
+    <row r="315" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E315" s="12"/>
+    </row>
+    <row r="316" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E316" s="12"/>
+    </row>
+    <row r="317" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E317" s="12"/>
+    </row>
+    <row r="318" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E318" s="12"/>
+    </row>
+    <row r="319" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E319" s="12"/>
+    </row>
+    <row r="320" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E320" s="12"/>
+    </row>
+    <row r="321" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E321" s="12"/>
+    </row>
+    <row r="322" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E322" s="12"/>
+    </row>
+    <row r="323" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E323" s="12"/>
+    </row>
+    <row r="324" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E324" s="12"/>
+    </row>
+    <row r="325" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E325" s="12"/>
+    </row>
+    <row r="326" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E326" s="12"/>
+    </row>
+    <row r="327" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E327" s="12"/>
+    </row>
+    <row r="328" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E328" s="12"/>
+    </row>
+    <row r="329" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E329" s="12"/>
+    </row>
+    <row r="330" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E330" s="12"/>
+    </row>
+    <row r="331" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E331" s="12"/>
+    </row>
+    <row r="332" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E332" s="12"/>
+    </row>
+    <row r="333" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E333" s="12"/>
+    </row>
+    <row r="334" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E334" s="12"/>
+    </row>
+    <row r="335" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E335" s="12"/>
+    </row>
+    <row r="336" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E336" s="12"/>
+    </row>
+    <row r="337" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E337" s="12"/>
+    </row>
+    <row r="338" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E338" s="12"/>
+    </row>
+    <row r="339" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E339" s="12"/>
+    </row>
+    <row r="340" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E340" s="12"/>
+    </row>
+    <row r="341" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E341" s="12"/>
+    </row>
+    <row r="342" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E342" s="12"/>
+    </row>
+    <row r="343" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E343" s="12"/>
+    </row>
+    <row r="344" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E344" s="12"/>
+    </row>
+    <row r="345" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E345" s="12"/>
+    </row>
+    <row r="346" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E346" s="12"/>
+    </row>
+    <row r="347" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E347" s="12"/>
+    </row>
+    <row r="348" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E348" s="12"/>
+    </row>
+    <row r="349" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E349" s="12"/>
+    </row>
+    <row r="350" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E350" s="12"/>
+    </row>
+    <row r="351" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E351" s="12"/>
+    </row>
+    <row r="352" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E352" s="12"/>
+    </row>
+    <row r="353" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E353" s="12"/>
+    </row>
+    <row r="354" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E354" s="12"/>
+    </row>
+    <row r="355" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E355" s="12"/>
+    </row>
+    <row r="356" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E356" s="12"/>
+    </row>
+    <row r="357" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E357" s="12"/>
+    </row>
+    <row r="358" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E358" s="12"/>
+    </row>
+    <row r="359" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E359" s="12"/>
+    </row>
+    <row r="360" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E360" s="12"/>
+    </row>
+    <row r="361" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E361" s="12"/>
+    </row>
+    <row r="362" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E362" s="12"/>
+    </row>
+    <row r="363" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E363" s="12"/>
+    </row>
+    <row r="364" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E364" s="12"/>
+    </row>
+    <row r="365" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E365" s="12"/>
+    </row>
+    <row r="366" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E366" s="12"/>
+    </row>
+    <row r="367" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E367" s="12"/>
+    </row>
+    <row r="368" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E368" s="12"/>
+    </row>
+    <row r="369" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E369" s="12"/>
+    </row>
+    <row r="370" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E370" s="12"/>
+    </row>
+    <row r="371" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E371" s="12"/>
+    </row>
+    <row r="372" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E372" s="12"/>
+    </row>
+    <row r="373" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E373" s="12"/>
+    </row>
+    <row r="374" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E374" s="12"/>
+    </row>
+    <row r="375" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E375" s="12"/>
+    </row>
+    <row r="376" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E376" s="12"/>
+    </row>
+    <row r="377" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E377" s="12"/>
+    </row>
+    <row r="378" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E378" s="12"/>
+    </row>
+    <row r="379" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E379" s="12"/>
+    </row>
+    <row r="380" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E380" s="12"/>
+    </row>
+    <row r="381" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E381" s="12"/>
+    </row>
+    <row r="382" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E382" s="12"/>
+    </row>
+    <row r="383" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E383" s="12"/>
+    </row>
+    <row r="384" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E384" s="12"/>
+    </row>
+    <row r="385" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E385" s="12"/>
+    </row>
+    <row r="386" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E386" s="12"/>
+    </row>
+    <row r="387" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E387" s="12"/>
+    </row>
+    <row r="388" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E388" s="12"/>
+    </row>
+    <row r="389" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E389" s="12"/>
+    </row>
+    <row r="390" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E390" s="12"/>
+    </row>
+    <row r="391" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E391" s="12"/>
+    </row>
+    <row r="392" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E392" s="12"/>
+    </row>
+    <row r="393" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E393" s="12"/>
+    </row>
+    <row r="394" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E394" s="12"/>
+    </row>
+    <row r="395" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E395" s="12"/>
+    </row>
+    <row r="396" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E396" s="12"/>
+    </row>
+    <row r="397" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E397" s="12"/>
+    </row>
+    <row r="398" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E398" s="12"/>
+    </row>
+    <row r="399" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E399" s="12"/>
+    </row>
+    <row r="400" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E400" s="12"/>
+    </row>
+    <row r="401" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E401" s="12"/>
+    </row>
+    <row r="402" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E402" s="12"/>
+    </row>
+    <row r="403" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E403" s="12"/>
+    </row>
+    <row r="404" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E404" s="12"/>
+    </row>
+    <row r="405" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E405" s="12"/>
+    </row>
+    <row r="406" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E406" s="12"/>
+    </row>
+    <row r="407" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E407" s="12"/>
+    </row>
+    <row r="408" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E408" s="12"/>
+    </row>
+    <row r="409" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E409" s="12"/>
+    </row>
+    <row r="410" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E410" s="12"/>
+    </row>
+    <row r="411" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E411" s="12"/>
+    </row>
+    <row r="412" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E412" s="12"/>
+    </row>
+    <row r="413" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E413" s="12"/>
+    </row>
+    <row r="414" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E414" s="12"/>
+    </row>
+    <row r="415" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E415" s="12"/>
+    </row>
+    <row r="416" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E416" s="12"/>
+    </row>
+    <row r="417" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E417" s="12"/>
+    </row>
+    <row r="418" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E418" s="12"/>
+    </row>
+    <row r="419" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E419" s="12"/>
+    </row>
+    <row r="420" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E420" s="12"/>
+    </row>
+    <row r="421" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E421" s="12"/>
+    </row>
+    <row r="422" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E422" s="12"/>
+    </row>
+    <row r="423" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E423" s="12"/>
+    </row>
+    <row r="424" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E424" s="12"/>
+    </row>
+    <row r="425" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E425" s="12"/>
+    </row>
+    <row r="426" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E426" s="12"/>
+    </row>
+    <row r="427" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E427" s="12"/>
+    </row>
+    <row r="428" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E428" s="12"/>
+    </row>
+    <row r="429" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E429" s="12"/>
+    </row>
+    <row r="430" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E430" s="12"/>
+    </row>
+    <row r="431" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E431" s="12"/>
+    </row>
+    <row r="432" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E432" s="12"/>
+    </row>
+    <row r="433" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E433" s="12"/>
+    </row>
+    <row r="434" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E434" s="12"/>
+    </row>
+    <row r="435" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E435" s="12"/>
+    </row>
+    <row r="436" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E436" s="12"/>
+    </row>
+    <row r="437" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E437" s="12"/>
+    </row>
+    <row r="438" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E438" s="12"/>
+    </row>
+    <row r="439" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E439" s="12"/>
+    </row>
+    <row r="440" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E440" s="12"/>
+    </row>
+    <row r="441" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E441" s="12"/>
+    </row>
+    <row r="442" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E442" s="12"/>
+    </row>
+    <row r="443" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E443" s="12"/>
+    </row>
+    <row r="444" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E444" s="12"/>
+    </row>
+    <row r="445" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E445" s="12"/>
+    </row>
+    <row r="446" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E446" s="12"/>
+    </row>
+    <row r="447" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E447" s="12"/>
+    </row>
+    <row r="448" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E448" s="12"/>
+    </row>
+    <row r="449" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E449" s="12"/>
+    </row>
+    <row r="450" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E450" s="12"/>
+    </row>
+    <row r="451" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E451" s="12"/>
+    </row>
+    <row r="452" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E452" s="12"/>
+    </row>
+    <row r="453" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E453" s="12"/>
+    </row>
+    <row r="454" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E454" s="12"/>
+    </row>
+    <row r="455" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E455" s="12"/>
+    </row>
+    <row r="456" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E456" s="12"/>
+    </row>
+    <row r="457" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E457" s="12"/>
+    </row>
+    <row r="458" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E458" s="12"/>
+    </row>
+    <row r="459" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E459" s="12"/>
+    </row>
+    <row r="460" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E460" s="12"/>
+    </row>
+    <row r="461" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E461" s="12"/>
+    </row>
+    <row r="462" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E462" s="12"/>
+    </row>
+    <row r="463" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E463" s="12"/>
+    </row>
+    <row r="464" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E464" s="12"/>
+    </row>
+    <row r="465" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E465" s="12"/>
+    </row>
+    <row r="466" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E466" s="12"/>
+    </row>
+    <row r="467" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E467" s="12"/>
+    </row>
+    <row r="468" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E468" s="12"/>
+    </row>
+    <row r="469" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E469" s="12"/>
+    </row>
+    <row r="470" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E470" s="12"/>
+    </row>
+    <row r="471" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E471" s="12"/>
+    </row>
+    <row r="472" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E472" s="12"/>
+    </row>
+    <row r="473" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E473" s="12"/>
+    </row>
+    <row r="474" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E474" s="12"/>
+    </row>
+    <row r="475" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E475" s="12"/>
+    </row>
+    <row r="476" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E476" s="12"/>
+    </row>
+    <row r="477" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E477" s="12"/>
+    </row>
+    <row r="478" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E478" s="12"/>
+    </row>
+    <row r="479" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E479" s="12"/>
+    </row>
+    <row r="480" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E480" s="12"/>
+    </row>
+    <row r="481" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E481" s="12"/>
+    </row>
+    <row r="482" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E482" s="12"/>
+    </row>
+    <row r="483" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E483" s="12"/>
+    </row>
+    <row r="484" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E484" s="12"/>
+    </row>
+    <row r="485" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E485" s="12"/>
+    </row>
+    <row r="486" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E486" s="12"/>
+    </row>
+    <row r="487" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E487" s="12"/>
+    </row>
+    <row r="488" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E488" s="12"/>
+    </row>
+    <row r="489" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E489" s="12"/>
+    </row>
+    <row r="490" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E490" s="12"/>
+    </row>
+    <row r="491" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E491" s="12"/>
+    </row>
+    <row r="492" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E492" s="12"/>
+    </row>
+    <row r="493" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E493" s="12"/>
+    </row>
+    <row r="494" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E494" s="12"/>
+    </row>
+    <row r="495" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E495" s="12"/>
+    </row>
+    <row r="496" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E496" s="12"/>
+    </row>
+    <row r="497" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E497" s="12"/>
+    </row>
+    <row r="498" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E498" s="12"/>
+    </row>
+    <row r="499" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E499" s="12"/>
+    </row>
+    <row r="500" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E500" s="12"/>
+    </row>
+    <row r="501" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E501" s="12"/>
+    </row>
+    <row r="502" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E502" s="12"/>
+    </row>
+    <row r="503" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E503" s="12"/>
+    </row>
+    <row r="504" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E504" s="12"/>
+    </row>
+    <row r="505" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E505" s="12"/>
+    </row>
+    <row r="506" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E506" s="12"/>
+    </row>
+    <row r="507" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E507" s="12"/>
+    </row>
+    <row r="508" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E508" s="12"/>
+    </row>
+    <row r="509" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E509" s="12"/>
+    </row>
+    <row r="510" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E510" s="12"/>
+    </row>
+    <row r="511" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E511" s="12"/>
+    </row>
+    <row r="512" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E512" s="12"/>
+    </row>
+    <row r="513" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E513" s="12"/>
+    </row>
+    <row r="514" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E514" s="12"/>
+    </row>
+    <row r="515" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E515" s="12"/>
     </row>
   </sheetData>
   <dataConsolidate/>
@@ -1116,7 +2773,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576">
       <formula1>"normal,low,high"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E515">
       <formula1>"to-do,in-progress,done"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Add RemoveText support for TextDocument
</commit_message>
<xml_diff>
--- a/docs/task-list.xlsx
+++ b/docs/task-list.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="38">
   <si>
     <t>Description</t>
   </si>
@@ -506,6 +506,18 @@
       </rPr>
       <t xml:space="preserve"> class</t>
     </r>
+  </si>
+  <si>
+    <t>Merge master-refactoring branch to master</t>
+  </si>
+  <si>
+    <t>Basically refactoring has been finished so two branches can be merged into one</t>
+  </si>
+  <si>
+    <t>Add grammar project to repository</t>
+  </si>
+  <si>
+    <t>CodeSharper grammar project should be attached to existing project</t>
   </si>
 </sst>
 </file>
@@ -963,7 +975,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -974,7 +986,7 @@
   <dimension ref="A1:G515"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1082,23 +1094,26 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+      <c r="A5" s="7">
         <v>4</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" s="3">
+      <c r="E5" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="11">
         <v>42044</v>
+      </c>
+      <c r="G5" s="11">
+        <v>42077</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1246,13 +1261,49 @@
       <c r="F12" s="11">
         <v>42070</v>
       </c>
-      <c r="G12" s="11"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E13" s="12"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E14" s="12"/>
+      <c r="G12" s="11">
+        <v>42070</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" s="3">
+        <v>42077</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F14" s="3">
+        <v>42077</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E15" s="12"/>

</xml_diff>

<commit_message>
Add Interpreter project to CodeSharper. Add CommandCall arguments (e.g.: NamedCommandCallActualArgument and PositionedCommandCallActualArgument classes).
</commit_message>
<xml_diff>
--- a/docs/task-list.xlsx
+++ b/docs/task-list.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="41">
   <si>
     <t>Description</t>
   </si>
@@ -518,6 +518,15 @@
   </si>
   <si>
     <t>CodeSharper grammar project should be attached to existing project</t>
+  </si>
+  <si>
+    <t>Implement CodeQuery language into project</t>
+  </si>
+  <si>
+    <t>CodeQuery language is ready, it is time to implement and migrate into the project</t>
+  </si>
+  <si>
+    <t>in-progress</t>
   </si>
 </sst>
 </file>
@@ -986,7 +995,7 @@
   <dimension ref="A1:G515"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1305,8 +1314,25 @@
         <v>42077</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E15" s="12"/>
+    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="F15" s="3">
+        <v>42077</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E16" s="12"/>

</xml_diff>

<commit_message>
Add selector descriptors and EqualityHelper class for implementing easily equality operators
</commit_message>
<xml_diff>
--- a/docs/task-list.xlsx
+++ b/docs/task-list.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="43">
   <si>
     <t>Description</t>
   </si>
@@ -527,6 +527,12 @@
   </si>
   <si>
     <t>in-progress</t>
+  </si>
+  <si>
+    <t>Implement selector language beside command calls</t>
+  </si>
+  <si>
+    <t>A selector language factory should be implemented</t>
   </si>
 </sst>
 </file>
@@ -984,7 +990,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -995,7 +1001,7 @@
   <dimension ref="A1:G515"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1334,8 +1340,25 @@
         <v>42077</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E16" s="12"/>
+    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F16" s="3">
+        <v>42077</v>
+      </c>
     </row>
     <row r="17" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E17" s="12"/>

</xml_diff>

<commit_message>
Add antlr grammars to project. Little refactoring in selectors.
</commit_message>
<xml_diff>
--- a/docs/task-list.xlsx
+++ b/docs/task-list.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="45">
   <si>
     <t>Description</t>
   </si>
@@ -529,10 +529,60 @@
     <t>in-progress</t>
   </si>
   <si>
-    <t>Implement selector language beside command calls</t>
-  </si>
-  <si>
     <t>A selector language factory should be implemented</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">[Selectors] </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Implement selector language beside command calls</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[Selectors]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Create a resolver class for building node operands, modifiers and selectors</t>
+    </r>
+  </si>
+  <si>
+    <t>There should be implemented a resolver class for creating node operands, modifiers and selectors</t>
   </si>
 </sst>
 </file>
@@ -990,7 +1040,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1001,7 +1051,7 @@
   <dimension ref="A1:G515"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1348,10 +1398,10 @@
         <v>12</v>
       </c>
       <c r="C16" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" s="4" t="s">
         <v>41</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>42</v>
       </c>
       <c r="E16" s="12" t="s">
         <v>16</v>
@@ -1360,52 +1410,69 @@
         <v>42077</v>
       </c>
     </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E17" s="12"/>
-    </row>
-    <row r="18" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F17" s="3">
+        <v>42078</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E18" s="12"/>
     </row>
-    <row r="19" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E19" s="12"/>
     </row>
-    <row r="20" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E20" s="12"/>
     </row>
-    <row r="21" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E21" s="12"/>
     </row>
-    <row r="22" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E22" s="12"/>
     </row>
-    <row r="23" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E23" s="12"/>
     </row>
-    <row r="24" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E24" s="12"/>
     </row>
-    <row r="25" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E25" s="12"/>
     </row>
-    <row r="26" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E26" s="12"/>
     </row>
-    <row r="27" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E27" s="12"/>
     </row>
-    <row r="28" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E28" s="12"/>
     </row>
-    <row r="29" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E29" s="12"/>
     </row>
-    <row r="30" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E30" s="12"/>
     </row>
-    <row r="31" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E31" s="12"/>
     </row>
-    <row r="32" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E32" s="12"/>
     </row>
     <row r="33" spans="5:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Rename nodes to more readable form. Implement CsvStandardSyntaxTreeBuilder class to support tree builder in more convenient way. Update task list.
</commit_message>
<xml_diff>
--- a/docs/task-list.xlsx
+++ b/docs/task-list.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="49">
   <si>
     <t>Description</t>
   </si>
@@ -366,9 +366,6 @@
     </r>
   </si>
   <si>
-    <t>Reconsider SelectRelativeNodesOperand implementation</t>
-  </si>
-  <si>
     <t>When algorithm finds a proper valid node it should not continue search in its children</t>
   </si>
   <si>
@@ -611,6 +608,168 @@
   </si>
   <si>
     <t>There should be dedicated node classes for representing CodeQuery language</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Reconsider </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>SelectRelativeNodesOperand</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> implementation</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[CSV]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Add more properties to Field and Row nodes</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">More properties should be added to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Field,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Row</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CsvDocument</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> nodes. For example there should be a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Rows</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> property of </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CsvDocument.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1068,7 +1227,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1078,8 +1237,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G515"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1283,10 +1442,10 @@
         <v>15</v>
       </c>
       <c r="C9" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>27</v>
       </c>
       <c r="E9" s="12" t="s">
         <v>16</v>
@@ -1303,10 +1462,10 @@
         <v>15</v>
       </c>
       <c r="C10" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>28</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>29</v>
       </c>
       <c r="E10" s="12" t="s">
         <v>16</v>
@@ -1323,10 +1482,10 @@
         <v>12</v>
       </c>
       <c r="C11" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>30</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>31</v>
       </c>
       <c r="E11" s="12" t="s">
         <v>16</v>
@@ -1343,10 +1502,10 @@
         <v>7</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E12" s="10" t="s">
         <v>14</v>
@@ -1366,10 +1525,10 @@
         <v>7</v>
       </c>
       <c r="C13" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="4" t="s">
         <v>34</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>35</v>
       </c>
       <c r="E13" s="12" t="s">
         <v>16</v>
@@ -1386,10 +1545,10 @@
         <v>7</v>
       </c>
       <c r="C14" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="4" t="s">
         <v>36</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>37</v>
       </c>
       <c r="E14" s="12" t="s">
         <v>16</v>
@@ -1406,13 +1565,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="E15" s="12" t="s">
         <v>39</v>
-      </c>
-      <c r="E15" s="12" t="s">
-        <v>40</v>
       </c>
       <c r="F15" s="3">
         <v>42077</v>
@@ -1426,10 +1585,10 @@
         <v>12</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E16" s="12" t="s">
         <v>16</v>
@@ -1446,10 +1605,10 @@
         <v>12</v>
       </c>
       <c r="C17" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" s="4" t="s">
         <v>43</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>44</v>
       </c>
       <c r="E17" s="12" t="s">
         <v>16</v>
@@ -1466,10 +1625,10 @@
         <v>7</v>
       </c>
       <c r="C18" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" s="4" t="s">
         <v>45</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>46</v>
       </c>
       <c r="E18" s="12" t="s">
         <v>16</v>
@@ -1478,8 +1637,25 @@
         <v>42078</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E19" s="12"/>
+    <row r="19" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F19" s="3">
+        <v>42085</v>
+      </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E20" s="12"/>

</xml_diff>

<commit_message>
Update and refactor some classes
</commit_message>
<xml_diff>
--- a/docs/task-list.xlsx
+++ b/docs/task-list.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="53">
   <si>
     <t>Description</t>
   </si>
@@ -770,6 +770,62 @@
       </rPr>
       <t>CsvDocument.</t>
     </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[Runnables]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Create RunnableFactory</t>
+    </r>
+  </si>
+  <si>
+    <t>RunnableFactory should be implemented like in ASP.NET MVC where ControllerFactory can be implemented in the framework</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">[Runnables] </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Implement SafeProofRunnable</t>
+    </r>
+  </si>
+  <si>
+    <t>There should be a "safe-proof" Runnable which encapsulates every Run() method with try-catch and logs any error</t>
   </si>
 </sst>
 </file>
@@ -1227,7 +1283,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1237,8 +1293,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G515"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1657,11 +1713,45 @@
         <v>42085</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E20" s="12"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E21" s="12"/>
+    <row r="20" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F20" s="3">
+        <v>42098</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>20</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E21" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F21" s="3">
+        <v>42098</v>
+      </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E22" s="12"/>

</xml_diff>

<commit_message>
Start to implement CodeQuery language and connect with control flows Update task list with new issues
</commit_message>
<xml_diff>
--- a/docs/task-list.xlsx
+++ b/docs/task-list.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="55">
   <si>
     <t>Description</t>
   </si>
@@ -826,6 +826,34 @@
   </si>
   <si>
     <t>There should be a "safe-proof" Runnable which encapsulates every Run() method with try-catch and logs any error</t>
+  </si>
+  <si>
+    <t>There should be an error-handling mechanism in control flows</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[Control Flows]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Add error handling to control flows</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1283,7 +1311,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1293,8 +1321,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G515"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1653,7 +1681,7 @@
         <v>42077</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1673,7 +1701,7 @@
         <v>42078</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -1693,7 +1721,7 @@
         <v>42078</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -1713,77 +1741,100 @@
         <v>42085</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
+    <row r="20" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="7">
         <v>19</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="D20" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="E20" s="12" t="s">
+      <c r="E20" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F20" s="11">
+        <v>42098</v>
+      </c>
+      <c r="G20" s="11">
+        <v>42104</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="7">
+        <v>20</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F21" s="11">
+        <v>42098</v>
+      </c>
+      <c r="G21" s="11">
+        <v>42104</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>21</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E22" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="F20" s="3">
-        <v>42098</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
-        <v>20</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="E21" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="F21" s="3">
-        <v>42098</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E22" s="12"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F22" s="3">
+        <v>42104</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E23" s="12"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E24" s="12"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E25" s="12"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E26" s="12"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E27" s="12"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E28" s="12"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E29" s="12"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E30" s="12"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E31" s="12"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E32" s="12"/>
     </row>
     <row r="33" spans="5:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Continue to implement command calls and convert to control flows.
</commit_message>
<xml_diff>
--- a/docs/task-list.xlsx
+++ b/docs/task-list.xlsx
@@ -1311,7 +1311,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1321,8 +1321,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G515"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>